<commit_message>
Final round of edits by Alejandro
I made a final round of edits based on a discussion with Micah. Waiting
for Eric´s final read and it will be ready to resubmit.
</commit_message>
<xml_diff>
--- a/papers/pygSpanish/Disponibilidad Info05.xlsx
+++ b/papers/pygSpanish/Disponibilidad Info05.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="68">
   <si>
     <t>Información</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>¿Su uso requiere herramienta? ¿cuál?</t>
-  </si>
-  <si>
-    <t>¿Herramienta disponible?</t>
   </si>
   <si>
     <t>Organo responsable</t>
@@ -379,12 +376,69 @@
       <t xml:space="preserve"> Plataforma de mapeo</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>¿Herramienta disponible?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>****</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">**** Herramienta disponible en </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">software </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">comercial y en </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">software </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>de código abierto.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -500,6 +554,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -533,8 +599,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -599,19 +671,25 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -944,7 +1022,7 @@
   <dimension ref="A1:AME48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="A1:H40"/>
+      <selection sqref="A1:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -955,7 +1033,7 @@
     <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
     <col min="9" max="1019" width="8.83203125" style="1"/>
   </cols>
@@ -980,15 +1058,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -1000,158 +1078,158 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1166,7 +1244,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
@@ -1178,106 +1256,106 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1292,7 +1370,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
@@ -1304,54 +1382,54 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1366,7 +1444,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -1378,80 +1456,80 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="G21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1466,7 +1544,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -1478,106 +1556,106 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H28" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1592,7 +1670,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
@@ -1604,28 +1682,28 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H32" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1640,7 +1718,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
@@ -1652,28 +1730,28 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="D35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H35" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1688,7 +1766,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -1700,7 +1778,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -1712,7 +1790,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -1724,7 +1802,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -1735,7 +1813,9 @@
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="7"/>
+      <c r="A41" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1789,12 +1869,12 @@
     </row>
     <row r="47" spans="1:8">
       <c r="F47" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="409">
       <c r="F48" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>